<commit_message>
Excel Change Because of Nainsi
</commit_message>
<xml_diff>
--- a/automation/Repository/Cancellation.xlsx
+++ b/automation/Repository/Cancellation.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Automation\automation\Repository\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18690" windowHeight="4935" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18690" windowHeight="4935"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="1" r:id="rId1"/>
@@ -18,6 +13,7 @@
     <sheet name="Error" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:R14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,13 +70,13 @@
     <t>cancdd</t>
   </si>
   <si>
-    <t>CS136744A9</t>
-  </si>
-  <si>
     <t>TEQJITIK</t>
   </si>
   <si>
     <t>H9007848A9</t>
+  </si>
+  <si>
+    <t>CE002662A9</t>
   </si>
 </sst>
 </file>
@@ -401,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +425,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -445,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -465,7 +461,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -473,7 +469,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -508,7 +504,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -516,7 +512,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Cancellation Test Condition 01
</commit_message>
<xml_diff>
--- a/automation/Repository/Cancellation.xlsx
+++ b/automation/Repository/Cancellation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Automation\Automation\automation\Repository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohit.goel\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>processed</t>
   </si>
@@ -87,9 +87,6 @@
     <t>VIN</t>
   </si>
   <si>
-    <t>ABCED</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -100,6 +97,18 @@
   </si>
   <si>
     <t>CERT</t>
+  </si>
+  <si>
+    <t>Vivek</t>
+  </si>
+  <si>
+    <t>Singla</t>
+  </si>
+  <si>
+    <t>20191411001</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -135,9 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,14 +472,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.7265625" bestFit="1" customWidth="1"/>
@@ -477,45 +488,57 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
+      <c r="C6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cancellation Test Condition 02 and 3
</commit_message>
<xml_diff>
--- a/automation/Repository/Cancellation.xlsx
+++ b/automation/Repository/Cancellation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohit.goel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Automation\Automation\automation\Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>processed</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>20191411001</t>
-  </si>
-  <si>
-    <t>v</t>
   </si>
 </sst>
 </file>
@@ -475,7 +472,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,12 +498,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>23</v>
       </c>
@@ -514,31 +511,25 @@
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
+      <c r="A6" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>